<commit_message>
complete renewal accordion kumap24a
</commit_message>
<xml_diff>
--- a/csvデータ配列早見表.xlsx
+++ b/csvデータ配列早見表.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadak\Desktop\trashmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadak\Desktop\読み上げ版\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E4DF36A-4006-48B2-84CE-72C7FF801913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5145D8BF-6343-4E66-90C6-EB470928734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7575" yWindow="1860" windowWidth="31320" windowHeight="19050" xr2:uid="{08EDF748-C5AF-4C03-AF76-D59289FD27CF}"/>
+    <workbookView xWindow="34950" yWindow="690" windowWidth="15555" windowHeight="20085" xr2:uid="{08EDF748-C5AF-4C03-AF76-D59289FD27CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>行政区</t>
   </si>
@@ -244,6 +244,10 @@
   </si>
   <si>
     <t>古紙衣類_14:30~16:30</t>
+  </si>
+  <si>
+    <t>備考</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -607,10 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F02AE34-8C7D-452F-A4BF-906CB424C923}">
-  <dimension ref="A1:B70"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -663,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -671,7 +676,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -679,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -687,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -695,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -703,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -711,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -719,7 +724,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -727,7 +732,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -735,7 +740,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -743,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -751,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -759,7 +764,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -767,7 +772,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -775,7 +780,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -783,7 +788,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -791,7 +796,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -799,7 +804,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -807,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -815,7 +820,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -823,7 +828,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -831,7 +836,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -839,7 +844,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -847,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -855,7 +860,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -863,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -871,7 +876,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -879,7 +884,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -887,7 +892,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -895,7 +900,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -903,7 +908,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -911,7 +916,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -919,7 +924,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -927,7 +932,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -935,7 +940,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -943,7 +948,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -951,7 +956,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -959,7 +964,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -967,7 +972,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -975,7 +980,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -983,7 +988,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -991,7 +996,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -999,7 +1004,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -1007,7 +1012,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -1015,7 +1020,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -1023,7 +1028,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -1031,7 +1036,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -1039,7 +1044,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -1047,7 +1052,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -1055,7 +1060,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -1063,7 +1068,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -1071,7 +1076,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -1079,7 +1084,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -1087,7 +1092,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -1095,7 +1100,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -1103,7 +1108,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -1111,7 +1116,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -1119,7 +1124,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -1127,7 +1132,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -1135,7 +1140,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -1143,7 +1148,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -1151,7 +1156,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -1159,7 +1164,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -1167,7 +1172,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -1175,6 +1180,14 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix kumap25 24 new Date
</commit_message>
<xml_diff>
--- a/csvデータ配列早見表.xlsx
+++ b/csvデータ配列早見表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadak\Desktop\読み上げ版\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tadak\Desktop\trashmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5145D8BF-6343-4E66-90C6-EB470928734D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514A499F-C820-4D48-B0C9-38009D92BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34950" yWindow="690" windowWidth="15555" windowHeight="20085" xr2:uid="{08EDF748-C5AF-4C03-AF76-D59289FD27CF}"/>
+    <workbookView xWindow="31545" yWindow="855" windowWidth="20025" windowHeight="20085" xr2:uid="{08EDF748-C5AF-4C03-AF76-D59289FD27CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,217 +36,237 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
-    <t>行政区</t>
-  </si>
-  <si>
-    <t>町名</t>
-  </si>
-  <si>
-    <t>丁目</t>
-  </si>
-  <si>
-    <t>番地</t>
+    <t>雑ごみ</t>
+  </si>
+  <si>
+    <t>普通ごみ_収集時間要問合せ</t>
+  </si>
+  <si>
+    <t>普通ごみ_午前</t>
+  </si>
+  <si>
+    <t>普通ごみ_午後</t>
+  </si>
+  <si>
+    <t>普通ごみ_8:30~10:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_9:00~11:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_9:30~11:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_10:00~12:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_10:30~12:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_11:00~13:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_11:30~13:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_12:00~14:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_12:30~14:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_13:00~15:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_13:30~15:30</t>
+  </si>
+  <si>
+    <t>普通ごみ_14:00~16:00</t>
+  </si>
+  <si>
+    <t>普通ごみ_14:30~16:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_収集時間要問合せ</t>
+  </si>
+  <si>
+    <t>資源ごみ_午前</t>
+  </si>
+  <si>
+    <t>資源ごみ_午後</t>
+  </si>
+  <si>
+    <t>資源ごみ_8:30~10:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_9:00~11:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_9:30~11:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_10:00~12:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_10:30~12:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_11:00~13:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_11:30~13:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_12:00~14:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_12:30~14:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_13:00~15:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_13:30~15:30</t>
+  </si>
+  <si>
+    <t>資源ごみ_14:00~16:00</t>
+  </si>
+  <si>
+    <t>資源ごみ_14:30~16:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_収集時間要問合せ</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_午前</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_午後</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_8:30~10:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_9:00~11:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_9:30~11:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_10:00~12:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_10:30~12:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_11:00~13:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_11:30~13:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_12:00~14:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_12:30~14:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_13:00~15:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_13:30~15:30</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_14:00~16:00</t>
+  </si>
+  <si>
+    <t>容器包装プラスチック_14:30~16:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_収集時間要問合せ</t>
+  </si>
+  <si>
+    <t>古紙衣類_午前</t>
+  </si>
+  <si>
+    <t>古紙衣類_午後</t>
+  </si>
+  <si>
+    <t>古紙衣類_8:30~10:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_9:00~11:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_9:30~11:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_10:00~12:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_10:30~12:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_11:00~13:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_11:30~13:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_12:00~14:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_12:30~14:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_13:00~15:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_13:30~15:30</t>
+  </si>
+  <si>
+    <t>古紙衣類_14:00~16:00</t>
+  </si>
+  <si>
+    <t>古紙衣類_14:30~16:30</t>
   </si>
   <si>
     <t>備考</t>
-  </si>
-  <si>
-    <t>雑ごみ</t>
-  </si>
-  <si>
-    <t>普通ごみ_収集時間要問合せ</t>
-  </si>
-  <si>
-    <t>普通ごみ_午前</t>
-  </si>
-  <si>
-    <t>普通ごみ_午後</t>
-  </si>
-  <si>
-    <t>普通ごみ_8:30~10:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_9:00~11:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_9:30~11:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_10:00~12:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_10:30~12:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_11:00~13:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_11:30~13:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_12:00~14:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_12:30~14:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_13:00~15:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_13:30~15:30</t>
-  </si>
-  <si>
-    <t>普通ごみ_14:00~16:00</t>
-  </si>
-  <si>
-    <t>普通ごみ_14:30~16:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_収集時間要問合せ</t>
-  </si>
-  <si>
-    <t>資源ごみ_午前</t>
-  </si>
-  <si>
-    <t>資源ごみ_午後</t>
-  </si>
-  <si>
-    <t>資源ごみ_8:30~10:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_9:00~11:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_9:30~11:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_10:00~12:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_10:30~12:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_11:00~13:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_11:30~13:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_12:00~14:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_12:30~14:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_13:00~15:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_13:30~15:30</t>
-  </si>
-  <si>
-    <t>資源ごみ_14:00~16:00</t>
-  </si>
-  <si>
-    <t>資源ごみ_14:30~16:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_収集時間要問合せ</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_午前</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_午後</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_8:30~10:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_9:00~11:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_9:30~11:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_10:00~12:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_10:30~12:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_11:00~13:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_11:30~13:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_12:00~14:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_12:30~14:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_13:00~15:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_13:30~15:30</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_14:00~16:00</t>
-  </si>
-  <si>
-    <t>容器包装プラスチック_14:30~16:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_収集時間要問合せ</t>
-  </si>
-  <si>
-    <t>古紙衣類_午前</t>
-  </si>
-  <si>
-    <t>古紙衣類_午後</t>
-  </si>
-  <si>
-    <t>古紙衣類_8:30~10:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_9:00~11:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_9:30~11:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_10:00~12:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_10:30~12:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_11:00~13:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_11:30~13:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_12:00~14:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_12:30~14:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_13:00~15:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_13:30~15:30</t>
-  </si>
-  <si>
-    <t>古紙衣類_14:00~16:00</t>
-  </si>
-  <si>
-    <t>古紙衣類_14:30~16:30</t>
-  </si>
-  <si>
-    <t>備考</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地区名１</t>
+    <rPh sb="0" eb="3">
+      <t>チクメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地区名２</t>
+    <rPh sb="0" eb="3">
+      <t>チクメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地区名３</t>
+    <rPh sb="0" eb="3">
+      <t>チクメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地区名４</t>
+    <rPh sb="0" eb="3">
+      <t>チクメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>地区名５</t>
+    <rPh sb="0" eb="3">
+      <t>チクメイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -614,8 +634,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -628,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -636,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -644,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -652,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -660,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -668,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -676,7 +696,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -684,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -692,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -700,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -708,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -716,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -724,7 +744,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -732,7 +752,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -740,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -748,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -756,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -764,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -772,7 +792,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -780,7 +800,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -788,7 +808,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -796,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -804,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -812,7 +832,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -820,7 +840,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -828,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -836,7 +856,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -844,7 +864,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -852,7 +872,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -860,7 +880,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -868,7 +888,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -876,7 +896,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -884,7 +904,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -892,7 +912,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -900,7 +920,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -908,7 +928,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -916,7 +936,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -924,7 +944,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -932,7 +952,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -940,7 +960,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -948,7 +968,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -956,7 +976,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -964,7 +984,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -972,7 +992,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -980,7 +1000,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -988,7 +1008,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -996,7 +1016,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -1004,7 +1024,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -1012,7 +1032,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -1020,7 +1040,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -1028,7 +1048,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -1036,7 +1056,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -1044,7 +1064,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -1052,7 +1072,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -1060,7 +1080,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -1068,7 +1088,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -1076,7 +1096,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -1084,7 +1104,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -1092,7 +1112,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -1100,7 +1120,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -1108,7 +1128,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -1116,7 +1136,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -1124,7 +1144,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -1132,7 +1152,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -1140,7 +1160,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -1148,7 +1168,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -1156,7 +1176,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -1164,7 +1184,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -1172,7 +1192,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -1180,7 +1200,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
@@ -1188,7 +1208,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>